<commit_message>
Fixed documentation bug (powered bit was in the wrong place). Implementation of said bit was also wrong in GCN_AdapterData. Fixed bug that was reading invalid memory in HID report generation (off by one error). Implemented null zone support for all analog inputs.
</commit_message>
<xml_diff>
--- a/docs/Gamecube controller data layout.xlsx
+++ b/docs/Gamecube controller data layout.xlsx
@@ -646,7 +646,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,8 +656,7 @@
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -707,10 +706,10 @@
       <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
       <c r="J3" t="s">
@@ -1345,5 +1344,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Previous commit was incorrect about the power bit changes in the documentation. Documentation has been reverted. Struct implementation of the power bit has been fixed.
</commit_message>
<xml_diff>
--- a/docs/Gamecube controller data layout.xlsx
+++ b/docs/Gamecube controller data layout.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gamecube controller data layout" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -646,7 +646,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,10 +706,10 @@
       <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
       <c r="J3" t="s">

</xml_diff>